<commit_message>
done with lab 6
</commit_message>
<xml_diff>
--- a/images/ZooChart.xlsx
+++ b/images/ZooChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie L\Projects\cf401\githubrepository\labs\lab05-06\zoo\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51C87B5-B009-4029-A1A0-92B4EC4C5E00}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2153141-58A0-4631-B695-A36CABBC50F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12435" windowHeight="4800" xr2:uid="{DC3C8A73-45BF-4F98-A4FF-DC3519E71FA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="55">
   <si>
     <t>Vertebrates</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>NumOfBabies</t>
+  </si>
+  <si>
+    <t>INTERFACE</t>
+  </si>
+  <si>
+    <t>Play()</t>
+  </si>
+  <si>
+    <t>SpeakInterface()</t>
+  </si>
+  <si>
+    <t>Pla()</t>
   </si>
 </sst>
 </file>
@@ -434,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -460,9 +472,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,13 +505,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -528,6 +530,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -846,10 +857,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AA54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,32 +899,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="J1" s="21"/>
-      <c r="K1" s="23" t="s">
+      <c r="J1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="19"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="4:20" x14ac:dyDescent="0.25">
       <c r="J2" s="5"/>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="4:20" x14ac:dyDescent="0.25">
       <c r="J3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>15</v>
       </c>
       <c r="L3" s="8"/>
@@ -937,7 +948,7 @@
     </row>
     <row r="5" spans="4:20" x14ac:dyDescent="0.25">
       <c r="J5" s="5"/>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="19" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="8"/>
@@ -948,7 +959,7 @@
       <c r="J6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="23" t="s">
         <v>46</v>
       </c>
       <c r="L6" s="8"/>
@@ -961,10 +972,10 @@
       <c r="J7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="7" t="s">
         <v>14</v>
       </c>
@@ -974,73 +985,73 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="17"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="17"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="14"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="13"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
     </row>
     <row r="10" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D10" s="21"/>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="19"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="23" t="s">
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="18"/>
+      <c r="P10" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="23"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="19"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="18"/>
     </row>
     <row r="11" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D11" s="5"/>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="H11" s="9"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="R11" s="24" t="s">
+      <c r="R11" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="S11" s="11" t="s">
+      <c r="S11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="T11" s="10"/>
+      <c r="T11" s="9"/>
     </row>
     <row r="12" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="8"/>
@@ -1051,7 +1062,7 @@
       <c r="P12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q12" s="20" t="s">
+      <c r="Q12" s="19" t="s">
         <v>15</v>
       </c>
       <c r="R12" s="8"/>
@@ -1114,14 +1125,14 @@
     </row>
     <row r="15" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="4"/>
       <c r="H15" s="8"/>
       <c r="P15" s="5"/>
-      <c r="Q15" s="20" t="s">
+      <c r="Q15" s="19" t="s">
         <v>16</v>
       </c>
       <c r="R15" s="8"/>
@@ -1132,7 +1143,7 @@
       <c r="D16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="23" t="s">
         <v>46</v>
       </c>
       <c r="F16" s="8" t="s">
@@ -1145,7 +1156,7 @@
       <c r="P16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="27" t="s">
+      <c r="Q16" s="23" t="s">
         <v>46</v>
       </c>
       <c r="R16" s="8" t="s">
@@ -1160,7 +1171,7 @@
       <c r="D17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="8"/>
@@ -1171,10 +1182,10 @@
       <c r="P17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Q17" s="15" t="s">
+      <c r="Q17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="R17" s="15" t="s">
+      <c r="R17" s="14" t="s">
         <v>2</v>
       </c>
       <c r="S17" s="7"/>
@@ -1184,129 +1195,129 @@
       <c r="D18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>2</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="8"/>
-      <c r="R18" s="26"/>
+      <c r="R18" s="22"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="14"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="14"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="13"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="14"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="23" t="s">
+      <c r="M20" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="O20" s="23"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="19"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="23" t="s">
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="18"/>
+      <c r="S20" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="U20" s="23"/>
-      <c r="V20" s="22"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="32"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="23" t="s">
+      <c r="A21" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="9"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="23" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="32"/>
+      <c r="G21" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="19"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="18"/>
       <c r="M21" s="5"/>
-      <c r="N21" s="24" t="s">
+      <c r="N21" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="O21" s="24" t="s">
+      <c r="O21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="P21" s="11" t="s">
+      <c r="P21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="Q21" s="10"/>
+      <c r="Q21" s="9"/>
       <c r="S21" s="5"/>
-      <c r="T21" s="24" t="s">
+      <c r="T21" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="U21" s="24" t="s">
+      <c r="U21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="V21" s="11" t="s">
+      <c r="V21" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>41</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="24" t="s">
+      <c r="I22" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="9"/>
       <c r="M22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="N22" s="19" t="s">
         <v>15</v>
       </c>
       <c r="O22" s="8"/>
       <c r="P22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q22" s="10"/>
+      <c r="Q22" s="9"/>
       <c r="S22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T22" s="20" t="s">
+      <c r="T22" s="19" t="s">
         <v>15</v>
       </c>
       <c r="U22" s="8"/>
@@ -1318,7 +1329,7 @@
       <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="8"/>
@@ -1328,14 +1339,14 @@
       <c r="G23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="19" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K23" s="10"/>
+      <c r="K23" s="9"/>
       <c r="M23" s="5" t="s">
         <v>24</v>
       </c>
@@ -1485,14 +1496,14 @@
       </c>
       <c r="K26" s="8"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="20" t="s">
+      <c r="N26" s="19" t="s">
         <v>16</v>
       </c>
       <c r="O26" s="8"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="8"/>
       <c r="S26" s="5"/>
-      <c r="T26" s="20" t="s">
+      <c r="T26" s="19" t="s">
         <v>16</v>
       </c>
       <c r="U26" s="8"/>
@@ -1500,13 +1511,13 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="4"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="19" t="s">
         <v>16</v>
       </c>
       <c r="I27" s="8"/>
@@ -1515,7 +1526,7 @@
       <c r="M27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N27" s="27" t="s">
+      <c r="N27" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O27" s="8" t="s">
@@ -1528,7 +1539,7 @@
       <c r="S27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="T27" s="27" t="s">
+      <c r="T27" s="23" t="s">
         <v>46</v>
       </c>
       <c r="U27" s="8" t="s">
@@ -1542,7 +1553,7 @@
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -1554,7 +1565,7 @@
       <c r="G28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="27" t="s">
+      <c r="H28" s="23" t="s">
         <v>46</v>
       </c>
       <c r="I28" s="8" t="s">
@@ -1567,10 +1578,10 @@
       <c r="M28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N28" s="15" t="s">
+      <c r="N28" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O28" s="15" t="s">
+      <c r="O28" s="14" t="s">
         <v>2</v>
       </c>
       <c r="P28" s="7" t="s">
@@ -1578,10 +1589,10 @@
       </c>
       <c r="Q28" s="8"/>
       <c r="S28" s="6"/>
-      <c r="T28" s="15" t="s">
+      <c r="T28" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="U28" s="15" t="s">
+      <c r="U28" s="14" t="s">
         <v>2</v>
       </c>
       <c r="V28" s="7" t="s">
@@ -1592,7 +1603,7 @@
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="23" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -1604,7 +1615,7 @@
       <c r="G29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="27" t="s">
+      <c r="H29" s="23" t="s">
         <v>47</v>
       </c>
       <c r="I29" s="8" t="s">
@@ -1614,17 +1625,17 @@
         <v>30</v>
       </c>
       <c r="K29" s="8"/>
-      <c r="O29" s="14"/>
+      <c r="O29" s="13"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
-      <c r="U29" s="18"/>
+      <c r="U29" s="17"/>
     </row>
     <row r="30" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="23" t="s">
         <v>48</v>
       </c>
       <c r="C30" s="8"/>
@@ -1634,23 +1645,23 @@
       <c r="G30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="14" t="s">
         <v>2</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K30" s="8"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="16"/>
-      <c r="U30" s="28"/>
-      <c r="V30" s="12"/>
-      <c r="W30" s="12"/>
-      <c r="X30" s="14"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="15"/>
+      <c r="U30" s="24"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="13"/>
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
       <c r="AA30" s="8"/>
@@ -1659,113 +1670,113 @@
       <c r="A31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I31" s="14"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="23" t="s">
+      <c r="M31" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="O31" s="23"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="30"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="23" t="s">
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="26"/>
+      <c r="S31" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="U31" s="23"/>
-      <c r="V31" s="22"/>
-      <c r="X31" s="14"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="32"/>
+      <c r="X31" s="13"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="14"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="8"/>
-      <c r="I32" s="14"/>
+      <c r="I32" s="13"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="24" t="s">
+      <c r="N32" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="O32" s="24" t="s">
+      <c r="O32" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="P32" s="11" t="s">
+      <c r="P32" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="Q32" s="31"/>
+      <c r="Q32" s="27"/>
       <c r="S32" s="5"/>
-      <c r="T32" s="24" t="s">
+      <c r="T32" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="U32" s="24" t="s">
+      <c r="U32" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="V32" s="11" t="s">
+      <c r="V32" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="X32" s="14"/>
+      <c r="X32" s="13"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="14"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="8"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="23" t="s">
+      <c r="G33" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="19"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="18"/>
       <c r="M33" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N33" s="20" t="s">
+      <c r="N33" s="19" t="s">
         <v>15</v>
       </c>
       <c r="O33" s="8"/>
       <c r="P33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q33" s="31"/>
+      <c r="Q33" s="27"/>
       <c r="S33" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T33" s="20" t="s">
+      <c r="T33" s="19" t="s">
         <v>15</v>
       </c>
       <c r="U33" s="8"/>
       <c r="V33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="X33" s="14"/>
+      <c r="X33" s="13"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="23" t="s">
+      <c r="A34" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="9"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="32"/>
       <c r="G34" s="5"/>
-      <c r="H34" s="24" t="s">
+      <c r="H34" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="24" t="s">
+      <c r="I34" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="J34" s="11" t="s">
+      <c r="J34" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K34" s="10"/>
+      <c r="K34" s="9"/>
       <c r="M34" s="5" t="s">
         <v>24</v>
       </c>
@@ -1778,7 +1789,7 @@
       <c r="P34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" s="17"/>
+      <c r="Q34" s="16"/>
       <c r="S34" s="5" t="s">
         <v>24</v>
       </c>
@@ -1791,23 +1802,23 @@
       <c r="V34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="X34" s="14"/>
+      <c r="X34" s="13"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>42</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="19" t="s">
         <v>15</v>
       </c>
       <c r="I35" s="8"/>
@@ -1827,7 +1838,7 @@
       <c r="P35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q35" s="17"/>
+      <c r="Q35" s="16"/>
       <c r="S35" s="5" t="s">
         <v>24</v>
       </c>
@@ -1840,13 +1851,13 @@
       <c r="V35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="X35" s="14"/>
+      <c r="X35" s="13"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="8"/>
@@ -1878,7 +1889,7 @@
       <c r="P36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q36" s="17"/>
+      <c r="Q36" s="16"/>
       <c r="S36" s="5" t="s">
         <v>24</v>
       </c>
@@ -1891,7 +1902,7 @@
       <c r="V36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="X36" s="14"/>
+      <c r="X36" s="13"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
@@ -1927,7 +1938,7 @@
       </c>
       <c r="O37" s="8"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="17"/>
+      <c r="Q37" s="16"/>
       <c r="S37" s="5" t="s">
         <v>24</v>
       </c>
@@ -1936,7 +1947,7 @@
       </c>
       <c r="U37" s="8"/>
       <c r="V37" s="4"/>
-      <c r="X37" s="14"/>
+      <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1965,19 +1976,19 @@
       </c>
       <c r="K38" s="8"/>
       <c r="M38" s="5"/>
-      <c r="N38" s="20" t="s">
+      <c r="N38" s="19" t="s">
         <v>16</v>
       </c>
       <c r="O38" s="8"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="17"/>
+      <c r="Q38" s="16"/>
       <c r="S38" s="5"/>
-      <c r="T38" s="20" t="s">
+      <c r="T38" s="19" t="s">
         <v>16</v>
       </c>
       <c r="U38" s="8"/>
       <c r="V38" s="4"/>
-      <c r="X38" s="14"/>
+      <c r="X38" s="13"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -2004,7 +2015,7 @@
       <c r="M39" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N39" s="27" t="s">
+      <c r="N39" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O39" s="8" t="s">
@@ -2013,11 +2024,11 @@
       <c r="P39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q39" s="17"/>
+      <c r="Q39" s="16"/>
       <c r="S39" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="T39" s="27" t="s">
+      <c r="T39" s="23" t="s">
         <v>46</v>
       </c>
       <c r="U39" s="8" t="s">
@@ -2026,50 +2037,46 @@
       <c r="V39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="X39" s="14"/>
-    </row>
-    <row r="40" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X39" s="13"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="4"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="19" t="s">
         <v>16</v>
       </c>
       <c r="I40" s="8"/>
       <c r="J40" s="4"/>
       <c r="K40" s="8"/>
-      <c r="M40" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N40" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="O40" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P40" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q40" s="17"/>
-      <c r="S40" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="T40" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="U40" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="V40" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="X40" s="14"/>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="M40" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N40" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O40" s="8"/>
+      <c r="P40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q40" s="16"/>
+      <c r="S40" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T40" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="U40" s="8"/>
+      <c r="V40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X40" s="13"/>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>28</v>
       </c>
@@ -2085,7 +2092,7 @@
       <c r="G41" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="27" t="s">
+      <c r="H41" s="23" t="s">
         <v>46</v>
       </c>
       <c r="I41" s="8" t="s">
@@ -2095,19 +2102,38 @@
         <v>34</v>
       </c>
       <c r="K41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="33"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="X41" s="14"/>
-    </row>
-    <row r="42" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O41" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P41" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q41" s="29"/>
+      <c r="S41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="U41" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="V41" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X41" s="13"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C42" s="8" t="s">
@@ -2117,30 +2143,29 @@
         <v>34</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H42" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>2</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I42" s="8"/>
       <c r="J42" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="K42" s="8"/>
+      <c r="N42" s="8"/>
       <c r="O42" s="28"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="12"/>
-      <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
+      <c r="P42" s="28"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="X42" s="13"/>
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="23" t="s">
         <v>47</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -2149,37 +2174,30 @@
       <c r="D43" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J43" s="7" t="s">
+      <c r="G43" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K43" s="8"/>
-      <c r="M43" s="21"/>
-      <c r="N43" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="O43" s="23"/>
-      <c r="P43" s="9"/>
-      <c r="S43" s="21"/>
-      <c r="T43" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="U43" s="23"/>
-      <c r="V43" s="22"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="O43" s="24"/>
+      <c r="T43" s="25"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+    </row>
+    <row r="44" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="23" t="s">
         <v>48</v>
       </c>
       <c r="C44" s="8" t="s">
@@ -2188,89 +2206,89 @@
       <c r="D44" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="G44" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="K44" s="2"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="O44" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="P44" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="S44" s="5"/>
-      <c r="T44" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="U44" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="V44" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="M44" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="N44" s="30"/>
+      <c r="O44" s="30"/>
+      <c r="P44" s="32"/>
+      <c r="S44" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="T44" s="30"/>
+      <c r="U44" s="30"/>
+      <c r="V44" s="32"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="15"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="7"/>
       <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
       <c r="K45" s="3"/>
-      <c r="M45" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="M45" s="5"/>
       <c r="N45" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="O45" s="8"/>
-      <c r="P45" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="S45" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="O45" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="S45" s="5"/>
       <c r="T45" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="U45" s="8"/>
-      <c r="V45" s="4" t="s">
-        <v>44</v>
+        <v>13</v>
+      </c>
+      <c r="U45" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="V45" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="M46" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N46" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O46" s="8" t="s">
-        <v>2</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="N46" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="O46" s="8"/>
       <c r="P46" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="S46" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="T46" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="U46" s="8" t="s">
-        <v>2</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="T46" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="U46" s="8"/>
       <c r="V46" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
@@ -2278,7 +2296,7 @@
         <v>24</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="O47" s="8" t="s">
         <v>2</v>
@@ -2290,7 +2308,7 @@
         <v>24</v>
       </c>
       <c r="T47" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="U47" s="8" t="s">
         <v>2</v>
@@ -2304,115 +2322,156 @@
         <v>24</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="O48" s="8" t="s">
         <v>2</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="S48" s="5" t="s">
         <v>24</v>
       </c>
       <c r="T48" s="8" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="U48" s="8" t="s">
         <v>2</v>
       </c>
       <c r="V48" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="13:22" x14ac:dyDescent="0.25">
       <c r="M49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N49" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O49" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T49" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="U49" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V49" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M50" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N49" s="8" t="s">
+      <c r="N50" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="O49" s="8"/>
-      <c r="P49" s="4"/>
-      <c r="S49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="T49" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="U49" s="8"/>
-      <c r="V49" s="4"/>
-    </row>
-    <row r="50" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M50" s="5"/>
-      <c r="N50" s="20" t="s">
-        <v>16</v>
       </c>
       <c r="O50" s="8"/>
       <c r="P50" s="4"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="20" t="s">
-        <v>16</v>
+      <c r="S50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T50" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="U50" s="8"/>
       <c r="V50" s="4"/>
     </row>
     <row r="51" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M51" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N51" s="27" t="s">
+      <c r="M51" s="5"/>
+      <c r="N51" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="O51" s="8"/>
+      <c r="P51" s="4"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="U51" s="8"/>
+      <c r="V51" s="4"/>
+    </row>
+    <row r="52" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M52" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N52" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="O51" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="P51" s="4" t="s">
+      <c r="O52" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P52" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S51" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="T51" s="27" t="s">
+      <c r="S52" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T52" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="U51" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="V51" s="4" t="s">
+      <c r="U52" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V52" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="13:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M52" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N52" s="15" t="s">
+    <row r="53" spans="13:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M53" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N53" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O52" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P52" s="7" t="s">
+      <c r="O53" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P53" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="S52" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="T52" s="15" t="s">
+      <c r="S53" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T53" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="U52" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="V52" s="7" t="s">
+      <c r="U53" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="V53" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="S53" s="2"/>
+    <row r="54" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="S54" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="S44:V44"/>
+    <mergeCell ref="S31:V31"/>
+    <mergeCell ref="M44:P44"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="M20:P20"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
finished updated interfaces for potty and play in peacock, goldfish and turtle
</commit_message>
<xml_diff>
--- a/images/ZooChart.xlsx
+++ b/images/ZooChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie L\Projects\cf401\githubrepository\labs\lab05-06\zoo\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2153141-58A0-4631-B695-A36CABBC50F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B49587B-1E73-4B79-BE71-8E0438549600}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12435" windowHeight="4800" xr2:uid="{DC3C8A73-45BF-4F98-A4FF-DC3519E71FA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="57">
   <si>
     <t>Vertebrates</t>
   </si>
@@ -183,13 +183,19 @@
     <t>INTERFACE</t>
   </si>
   <si>
-    <t>Play()</t>
-  </si>
-  <si>
-    <t>SpeakInterface()</t>
-  </si>
-  <si>
-    <t>Pla()</t>
+    <t>PottyInterface()</t>
+  </si>
+  <si>
+    <t>PlayInterface()</t>
+  </si>
+  <si>
+    <t>Interface - Iplay</t>
+  </si>
+  <si>
+    <t>Interface - Ipotty</t>
+  </si>
+  <si>
+    <t>PlayInterface</t>
   </si>
 </sst>
 </file>
@@ -237,7 +243,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -423,18 +429,31 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -446,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -519,26 +538,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -857,31 +873,31 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA54"/>
+  <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -899,12 +915,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="32"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="28"/>
       <c r="N1" s="18"/>
     </row>
     <row r="2" spans="4:20" x14ac:dyDescent="0.25">
@@ -1006,19 +1022,19 @@
       <c r="T9" s="8"/>
     </row>
     <row r="10" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="32"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="18"/>
-      <c r="P10" s="31" t="s">
+      <c r="P10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="32"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="28"/>
       <c r="T10" s="18"/>
     </row>
     <row r="11" spans="4:20" x14ac:dyDescent="0.25">
@@ -1231,33 +1247,33 @@
       <c r="I20" s="13"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-      <c r="M20" s="31" t="s">
+      <c r="M20" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="32"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="28"/>
       <c r="Q20" s="18"/>
-      <c r="S20" s="31" t="s">
+      <c r="S20" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="32"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="28"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="32"/>
-      <c r="G21" s="31" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="G21" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="32"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
       <c r="K21" s="18"/>
       <c r="M21" s="5"/>
       <c r="N21" s="20" t="s">
@@ -1625,7 +1641,7 @@
         <v>30</v>
       </c>
       <c r="K29" s="8"/>
-      <c r="O29" s="13"/>
+      <c r="O29" s="17"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
@@ -1655,9 +1671,13 @@
         <v>14</v>
       </c>
       <c r="K30" s="8"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="15"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
       <c r="U30" s="24"/>
       <c r="V30" s="11"/>
       <c r="W30" s="11"/>
@@ -1682,19 +1702,21 @@
       <c r="I31" s="13"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="M31" s="31" t="s">
+      <c r="L31" s="13"/>
+      <c r="M31" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="26"/>
-      <c r="S31" s="31" t="s">
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="32"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="28"/>
       <c r="X31" s="13"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1703,6 +1725,7 @@
       <c r="I32" s="13"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
+      <c r="L32" s="13"/>
       <c r="M32" s="5"/>
       <c r="N32" s="20" t="s">
         <v>13</v>
@@ -1713,7 +1736,8 @@
       <c r="P32" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="Q32" s="27"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="8"/>
       <c r="S32" s="5"/>
       <c r="T32" s="20" t="s">
         <v>13</v>
@@ -1729,13 +1753,14 @@
     <row r="33" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="13"/>
       <c r="D33" s="8"/>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="32"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
       <c r="K33" s="18"/>
+      <c r="L33" s="13"/>
       <c r="M33" s="5" t="s">
         <v>43</v>
       </c>
@@ -1746,7 +1771,8 @@
       <c r="P33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q33" s="27"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="8"/>
       <c r="S33" s="5" t="s">
         <v>43</v>
       </c>
@@ -1760,12 +1786,12 @@
       <c r="X33" s="13"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="32"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
       <c r="G34" s="5"/>
       <c r="H34" s="20" t="s">
         <v>13</v>
@@ -1777,6 +1803,7 @@
         <v>42</v>
       </c>
       <c r="K34" s="9"/>
+      <c r="L34" s="13"/>
       <c r="M34" s="5" t="s">
         <v>24</v>
       </c>
@@ -1789,7 +1816,8 @@
       <c r="P34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" s="16"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
       <c r="S34" s="5" t="s">
         <v>24</v>
       </c>
@@ -1826,6 +1854,7 @@
         <v>44</v>
       </c>
       <c r="K35" s="8"/>
+      <c r="L35" s="13"/>
       <c r="M35" s="5" t="s">
         <v>24</v>
       </c>
@@ -1838,7 +1867,8 @@
       <c r="P35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q35" s="16"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
       <c r="S35" s="5" t="s">
         <v>24</v>
       </c>
@@ -1877,6 +1907,7 @@
         <v>30</v>
       </c>
       <c r="K36" s="8"/>
+      <c r="L36" s="13"/>
       <c r="M36" s="5" t="s">
         <v>24</v>
       </c>
@@ -1889,7 +1920,8 @@
       <c r="P36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q36" s="16"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
       <c r="S36" s="5" t="s">
         <v>24</v>
       </c>
@@ -1930,6 +1962,7 @@
         <v>34</v>
       </c>
       <c r="K37" s="8"/>
+      <c r="L37" s="13"/>
       <c r="M37" s="5" t="s">
         <v>24</v>
       </c>
@@ -1938,7 +1971,8 @@
       </c>
       <c r="O37" s="8"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="16"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
       <c r="S37" s="5" t="s">
         <v>24</v>
       </c>
@@ -1975,13 +2009,15 @@
         <v>34</v>
       </c>
       <c r="K38" s="8"/>
+      <c r="L38" s="13"/>
       <c r="M38" s="5"/>
       <c r="N38" s="19" t="s">
         <v>16</v>
       </c>
       <c r="O38" s="8"/>
       <c r="P38" s="4"/>
-      <c r="Q38" s="16"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
       <c r="S38" s="5"/>
       <c r="T38" s="19" t="s">
         <v>16</v>
@@ -2012,6 +2048,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="4"/>
       <c r="K39" s="8"/>
+      <c r="L39" s="13"/>
       <c r="M39" s="5" t="s">
         <v>28</v>
       </c>
@@ -2024,7 +2061,8 @@
       <c r="P39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Q39" s="16"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
       <c r="S39" s="5" t="s">
         <v>28</v>
       </c>
@@ -2053,22 +2091,24 @@
       <c r="I40" s="8"/>
       <c r="J40" s="4"/>
       <c r="K40" s="8"/>
+      <c r="L40" s="13"/>
       <c r="M40" s="5" t="s">
         <v>31</v>
       </c>
       <c r="N40" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O40" s="8"/>
       <c r="P40" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="Q40" s="16"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="12"/>
       <c r="S40" s="5" t="s">
         <v>31</v>
       </c>
       <c r="T40" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U40" s="8"/>
       <c r="V40" s="4" t="s">
@@ -2102,6 +2142,7 @@
         <v>34</v>
       </c>
       <c r="K41" s="8"/>
+      <c r="L41" s="13"/>
       <c r="M41" s="6" t="s">
         <v>28</v>
       </c>
@@ -2114,7 +2155,8 @@
       <c r="P41" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Q41" s="29"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="13"/>
       <c r="S41" s="6" t="s">
         <v>28</v>
       </c>
@@ -2142,20 +2184,24 @@
       <c r="D42" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="F42" s="30"/>
       <c r="G42" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H42" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I42" s="8"/>
       <c r="J42" s="4" t="s">
         <v>51</v>
       </c>
       <c r="K42" s="8"/>
+      <c r="L42" s="31"/>
       <c r="N42" s="8"/>
-      <c r="O42" s="28"/>
-      <c r="P42" s="28"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="13"/>
       <c r="U42" s="8"/>
       <c r="V42" s="8"/>
       <c r="X42" s="13"/>
@@ -2174,6 +2220,7 @@
       <c r="D43" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="F43" s="13"/>
       <c r="G43" s="5" t="s">
         <v>28</v>
       </c>
@@ -2187,7 +2234,13 @@
         <v>34</v>
       </c>
       <c r="K43" s="8"/>
-      <c r="O43" s="24"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="13"/>
       <c r="T43" s="25"/>
       <c r="U43" s="11"/>
       <c r="V43" s="11"/>
@@ -2206,6 +2259,7 @@
       <c r="D44" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="F44" s="13"/>
       <c r="G44" s="6" t="s">
         <v>28</v>
       </c>
@@ -2219,18 +2273,19 @@
         <v>34</v>
       </c>
       <c r="K44" s="2"/>
-      <c r="M44" s="31" t="s">
+      <c r="M44" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="32"/>
-      <c r="S44" s="31" t="s">
+      <c r="N44" s="27"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="28"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="T44" s="30"/>
-      <c r="U44" s="30"/>
-      <c r="V44" s="32"/>
+      <c r="T44" s="27"/>
+      <c r="U44" s="27"/>
+      <c r="V44" s="28"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
@@ -2241,7 +2296,7 @@
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="7"/>
-      <c r="F45" s="8"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
@@ -2256,6 +2311,7 @@
       <c r="P45" s="10" t="s">
         <v>42</v>
       </c>
+      <c r="R45" s="13"/>
       <c r="S45" s="5"/>
       <c r="T45" s="20" t="s">
         <v>13</v>
@@ -2270,6 +2326,7 @@
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
+      <c r="F46" s="13"/>
       <c r="M46" s="5" t="s">
         <v>43</v>
       </c>
@@ -2280,6 +2337,7 @@
       <c r="P46" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="R46" s="13"/>
       <c r="S46" s="5" t="s">
         <v>43</v>
       </c>
@@ -2292,6 +2350,7 @@
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F47" s="13"/>
       <c r="M47" s="5" t="s">
         <v>24</v>
       </c>
@@ -2304,6 +2363,7 @@
       <c r="P47" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="R47" s="13"/>
       <c r="S47" s="5" t="s">
         <v>24</v>
       </c>
@@ -2318,6 +2378,7 @@
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F48" s="13"/>
       <c r="M48" s="5" t="s">
         <v>24</v>
       </c>
@@ -2330,6 +2391,7 @@
       <c r="P48" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="R48" s="13"/>
       <c r="S48" s="5" t="s">
         <v>24</v>
       </c>
@@ -2343,7 +2405,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="13:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F49" s="13"/>
       <c r="M49" s="5" t="s">
         <v>24</v>
       </c>
@@ -2356,6 +2419,7 @@
       <c r="P49" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="R49" s="13"/>
       <c r="S49" s="5" t="s">
         <v>24</v>
       </c>
@@ -2369,7 +2433,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="13:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F50" s="13"/>
       <c r="M50" s="5" t="s">
         <v>31</v>
       </c>
@@ -2378,6 +2443,7 @@
       </c>
       <c r="O50" s="8"/>
       <c r="P50" s="4"/>
+      <c r="R50" s="13"/>
       <c r="S50" s="5" t="s">
         <v>25</v>
       </c>
@@ -2387,13 +2453,15 @@
       <c r="U50" s="8"/>
       <c r="V50" s="4"/>
     </row>
-    <row r="51" spans="13:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F51" s="13"/>
       <c r="M51" s="5"/>
       <c r="N51" s="19" t="s">
         <v>16</v>
       </c>
       <c r="O51" s="8"/>
       <c r="P51" s="4"/>
+      <c r="R51" s="13"/>
       <c r="S51" s="5"/>
       <c r="T51" s="19" t="s">
         <v>16</v>
@@ -2401,7 +2469,8 @@
       <c r="U51" s="8"/>
       <c r="V51" s="4"/>
     </row>
-    <row r="52" spans="13:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F52" s="13"/>
       <c r="M52" s="5" t="s">
         <v>28</v>
       </c>
@@ -2414,6 +2483,7 @@
       <c r="P52" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="R52" s="13"/>
       <c r="S52" s="5" t="s">
         <v>28</v>
       </c>
@@ -2427,7 +2497,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="13:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="13"/>
       <c r="M53" s="6" t="s">
         <v>28</v>
       </c>
@@ -2440,6 +2511,7 @@
       <c r="P53" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="R53" s="13"/>
       <c r="S53" s="6" t="s">
         <v>28</v>
       </c>
@@ -2453,11 +2525,55 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="13:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F54" s="13"/>
+      <c r="R54" s="13"/>
       <c r="S54" s="2"/>
     </row>
+    <row r="55" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F55" s="13"/>
+      <c r="R55" s="13"/>
+    </row>
+    <row r="56" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="F56" s="13"/>
+      <c r="R56" s="13"/>
+    </row>
+    <row r="57" spans="5:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F57" s="29"/>
+      <c r="R57" s="29"/>
+    </row>
+    <row r="58" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E58" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F58" s="28"/>
+      <c r="Q58" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="R58" s="28"/>
+    </row>
+    <row r="59" spans="5:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E59" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q59" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="S44:V44"/>
+    <mergeCell ref="S31:V31"/>
+    <mergeCell ref="M44:P44"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="S20:V20"/>
+    <mergeCell ref="M20:P20"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="P10:S10"/>
     <mergeCell ref="J1:M1"/>
@@ -2465,12 +2581,8 @@
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="G33:J33"/>
-    <mergeCell ref="S44:V44"/>
-    <mergeCell ref="S31:V31"/>
-    <mergeCell ref="M44:P44"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="S20:V20"/>
-    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="Q58:R58"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="landscape" r:id="rId1"/>

</xml_diff>